<commit_message>
report PDF : change procedure
</commit_message>
<xml_diff>
--- a/templates/postReport.xlsx
+++ b/templates/postReport.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678A6316-EC08-4EE7-A9DE-0730AC049DF9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BADE50-E728-483B-BC81-2DD77AE26E08}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,9 +190,6 @@
     <t>TC</t>
   </si>
   <si>
-    <t>Soudure Inertiel</t>
-  </si>
-  <si>
     <t>Position de la fissure</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>Position de l'initiation</t>
+  </si>
+  <si>
+    <t>Soudure Inertie</t>
   </si>
 </sst>
 </file>
@@ -293,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +397,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="48"/>
+      <color rgb="FF8193AB"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -457,7 +463,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -506,6 +512,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1005,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1057,65 +1066,65 @@
     </row>
     <row r="4" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="18" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1124,34 +1133,34 @@
       <c r="D7" s="15"/>
       <c r="E7" s="14"/>
       <c r="F7" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>42</v>
-      </c>
       <c r="D8" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="18" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1169,10 +1178,10 @@
         <v>19</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1190,10 +1199,10 @@
         <v>23</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1204,17 +1213,17 @@
         <v>34</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1225,17 +1234,17 @@
         <v>35</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="18" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -1246,7 +1255,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="6"/>
@@ -1329,8 +1338,8 @@
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:9" s="11" customFormat="1" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A34" s="20" t="s">
-        <v>51</v>
+      <c r="A34" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>

</xml_diff>

<commit_message>
post report : add FOL
</commit_message>
<xml_diff>
--- a/templates/postReport.xlsx
+++ b/templates/postReport.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213B69A2-D642-42BE-BFD3-837ABBE038FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14523C4A-F2BF-4285-85B1-2287D66CA7D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5460" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32925" yWindow="-2940" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="En-tête" sheetId="14" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>Rapport d'essai</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Filets</t>
   </si>
   <si>
-    <t>Rayon</t>
-  </si>
-  <si>
     <t>Couteaux Extensomètre</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>Button</t>
   </si>
   <si>
-    <t>At Radius</t>
-  </si>
-  <si>
     <t>At eXtensometer probes</t>
   </si>
   <si>
@@ -286,7 +280,37 @@
     <t>Soudure Inertie</t>
   </si>
   <si>
-    <t>AR / RAD</t>
+    <t>FOL</t>
+  </si>
+  <si>
+    <t>Fracture avant atteinte max</t>
+  </si>
+  <si>
+    <t>Failure On Loading (before max)</t>
+  </si>
+  <si>
+    <t>IR/RAD</t>
+  </si>
+  <si>
+    <t>In the Radius</t>
+  </si>
+  <si>
+    <t>G/GAGE</t>
+  </si>
+  <si>
+    <t>Gage Section</t>
+  </si>
+  <si>
+    <t>Dans le Rayon</t>
+  </si>
+  <si>
+    <t>At transition gage-Radius</t>
+  </si>
+  <si>
+    <t>Partie Calibrée</t>
+  </si>
+  <si>
+    <t>A transition partie calibrée-Rayon</t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1072,10 +1096,10 @@
         <v>40</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="16" t="s">
@@ -1085,7 +1109,7 @@
         <v>39</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1106,7 +1130,7 @@
         <v>51</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1117,17 +1141,17 @@
         <v>48</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="18" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1153,7 +1177,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="18" t="s">
@@ -1178,13 +1202,13 @@
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="18" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1199,13 +1223,13 @@
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="18" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -1216,63 +1240,81 @@
         <v>34</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G13" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
+      <c r="H13" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:9" s="13" customFormat="1" ht="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>